<commit_message>
Add NOAA-20 to platform, update mappings, add VIIRS product strings
</commit_message>
<xml_diff>
--- a/data/cci/cci-platform-programme-mapping.xlsx
+++ b/data/cci/cci-platform-programme-mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amw23\Documents\GitHub\cci-vocabularies\data\cci\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsl11288\DOCUME~1\Moba\slash\RemoteFiles\262446_2_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B578D75-0C86-42DE-B89F-E3A99152975E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFFCBF6-AA4F-4E3F-8EBA-4AA3B5070369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{D6294A95-F961-1A4F-9365-26DAE540CA74}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{D6294A95-F961-1A4F-9365-26DAE540CA74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="237">
   <si>
     <t>URI 1</t>
   </si>
@@ -752,6 +752,9 @@
   </si>
   <si>
     <t>plat_iss_prog</t>
+  </si>
+  <si>
+    <t>plat_noaa_20</t>
   </si>
 </sst>
 </file>
@@ -2407,19 +2410,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DF6A92B-36B9-F243-89DF-2828BF9C02CE}">
-  <dimension ref="A1:D173"/>
+  <dimension ref="A1:D174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="D173" sqref="D173"/>
+    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="C179" sqref="C179"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="34.85546875" customWidth="1"/>
-    <col min="5" max="64" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25.26953125" customWidth="1"/>
+    <col min="2" max="2" width="31.7265625" customWidth="1"/>
+    <col min="3" max="3" width="22.7265625" customWidth="1"/>
+    <col min="4" max="4" width="34.81640625" customWidth="1"/>
+    <col min="5" max="64" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3836,7 +3839,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="17.25">
+    <row r="102" spans="1:4" ht="16.5">
       <c r="A102" s="4" t="s">
         <v>130</v>
       </c>
@@ -3850,7 +3853,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="17.25">
+    <row r="103" spans="1:4" ht="16.5">
       <c r="A103" s="4" t="s">
         <v>130</v>
       </c>
@@ -3864,7 +3867,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="17.25">
+    <row r="104" spans="1:4" ht="16.5">
       <c r="A104" s="4" t="s">
         <v>130</v>
       </c>
@@ -3878,7 +3881,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="17.25">
+    <row r="105" spans="1:4" ht="16.5">
       <c r="A105" s="4" t="s">
         <v>130</v>
       </c>
@@ -3892,7 +3895,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="17.25">
+    <row r="106" spans="1:4" ht="16.5">
       <c r="A106" s="4" t="s">
         <v>130</v>
       </c>
@@ -3906,7 +3909,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="17.25">
+    <row r="107" spans="1:4" ht="16.5">
       <c r="A107" s="4" t="s">
         <v>130</v>
       </c>
@@ -3920,7 +3923,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="17.25">
+    <row r="108" spans="1:4" ht="16.5">
       <c r="A108" s="4" t="s">
         <v>130</v>
       </c>
@@ -3934,7 +3937,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="17.25">
+    <row r="109" spans="1:4" ht="16.5">
       <c r="A109" s="4" t="s">
         <v>130</v>
       </c>
@@ -3948,7 +3951,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="17.25">
+    <row r="110" spans="1:4" ht="16.5">
       <c r="A110" s="4" t="s">
         <v>130</v>
       </c>
@@ -3962,7 +3965,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="17.25">
+    <row r="111" spans="1:4" ht="16.5">
       <c r="A111" s="3" t="s">
         <v>140</v>
       </c>
@@ -3976,7 +3979,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="17.25">
+    <row r="112" spans="1:4" ht="16.5">
       <c r="A112" s="3" t="s">
         <v>140</v>
       </c>
@@ -3990,7 +3993,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="17.25">
+    <row r="113" spans="1:4" ht="16.5">
       <c r="A113" s="3" t="s">
         <v>140</v>
       </c>
@@ -4004,7 +4007,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="17.25">
+    <row r="114" spans="1:4" ht="16.5">
       <c r="A114" s="3" t="s">
         <v>140</v>
       </c>
@@ -4018,7 +4021,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="17.25">
+    <row r="115" spans="1:4" ht="16.5">
       <c r="A115" s="3" t="s">
         <v>140</v>
       </c>
@@ -4841,6 +4844,20 @@
         <v>234</v>
       </c>
       <c r="D173" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174" t="s">
+        <v>187</v>
+      </c>
+      <c r="B174" t="s">
+        <v>5</v>
+      </c>
+      <c r="C174" t="s">
+        <v>236</v>
+      </c>
+      <c r="D174" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>